<commit_message>
finished all card types
</commit_message>
<xml_diff>
--- a/tactics.xlsx
+++ b/tactics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I852780\Desktop\football team\footballteam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfc90\Desktop\Footballteam\footballteam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0529C09D-3155-43BF-AE34-B91C0D82363D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECB5898-7257-4E3C-94DF-68E417453C6A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{6ACF284B-7517-4806-93BB-B0394A55D5D8}"/>
   </bookViews>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -410,7 +410,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>